<commit_message>
Small schedule edits plus removing auxiliary files from repository
</commit_message>
<xml_diff>
--- a/Schedule_Oberwolfach2413/Oberwolfach_2413_ScheduleOverview.xlsx
+++ b/Schedule_Oberwolfach2413/Oberwolfach_2413_ScheduleOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\WorkshopsConferencesEvents\Oberwolfach2413_ScheduleAndReport\Schedule_Oberwolfach2413\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94042657-A31F-4A96-B8F2-0154A72F1B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3115E0A-20C5-4763-8F90-B43EB59B9C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
   <si>
     <t>Other</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>Algebraic proof complexity of tensors</t>
+  </si>
+  <si>
+    <t>Open problems session?</t>
+  </si>
+  <si>
+    <t>Music evening?</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -489,11 +495,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -587,6 +608,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -893,10 +917,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,37 +1710,62 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="7">
+        <v>0.80208333333334303</v>
+      </c>
       <c r="B46" s="14"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="14"/>
+      <c r="G46" s="7">
+        <v>0.80208333333334303</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="7">
+        <v>0.81250000000000999</v>
+      </c>
       <c r="B47" s="14"/>
       <c r="F47" s="1"/>
+      <c r="G47" s="7">
+        <v>0.81250000000000999</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="7">
+        <v>0.82291666666667695</v>
+      </c>
       <c r="B48" s="8"/>
       <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="G48" s="7">
+        <v>0.82291666666667695</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>0.83333333333334403</v>
+      </c>
       <c r="B49" s="13"/>
+      <c r="C49" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>88</v>
+      </c>
       <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="7">
+        <v>0.83333333333334403</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.6692913385826772" right="0.6692913385826772" top="0.39370078740157483" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="75" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>